<commit_message>
Pressure config 6 & interior pressure mapping
</commit_message>
<xml_diff>
--- a/Measurements/template_mastersheet.xlsx
+++ b/Measurements/template_mastersheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michiel/Dimple - Working Documents/DimpleTech/10 Technology development/01 The Hill/03 Usage/Measurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A250AAC-EF32-6B4C-B291-0EDEA4FC1C45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD30F57-78B5-F144-AC10-56D3FCC6926D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19600" activeTab="2" xr2:uid="{E12EEECC-AC3A-F945-9F00-751131698F74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19600" xr2:uid="{E12EEECC-AC3A-F945-9F00-751131698F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD142BB9-230F-7B49-905A-C5597AFD6720}">
   <dimension ref="B1:P179"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1232,7 +1232,7 @@
         <v>34</v>
       </c>
       <c r="M4" s="28" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="N4" s="50"/>
       <c r="O4" s="52"/>
@@ -3030,7 +3030,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE1AFB58-885D-224A-A057-9669FDA4BA0C}">
           <x14:formula1>
-            <xm:f>'Pressure layouts'!$I$2:$M$2</xm:f>
+            <xm:f>'Pressure layouts'!$I$2:$N$2</xm:f>
           </x14:formula1>
           <xm:sqref>M4:M179</xm:sqref>
         </x14:dataValidation>
@@ -3106,7 +3106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A10DB1-E37C-5244-B63B-8274B8B3FC20}">
   <dimension ref="B1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>

</xml_diff>